<commit_message>
Implementacion de Dublin core
</commit_message>
<xml_diff>
--- a/data/BGA-obra.xlsx
+++ b/data/BGA-obra.xlsx
@@ -10,7 +10,6 @@
   <sheets>
     <sheet name="referente" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="obra" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="bga-obra" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,18 +21,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
   <si>
-    <t xml:space="preserve">titulo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fecha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">periodico</t>
+    <t xml:space="preserve">title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">publisher</t>
   </si>
   <si>
     <t xml:space="preserve">archivo</t>
@@ -69,10 +68,10 @@
     <t xml:space="preserve">exmilitar-mata-esposa.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">dimensiones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tecnica</t>
+    <t xml:space="preserve">format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">medium</t>
   </si>
   <si>
     <t xml:space="preserve">Los Suicidas del Sisga No 1</t>
@@ -221,7 +220,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -325,8 +324,8 @@
   </sheetPr>
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -439,177 +438,4 @@
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:G8"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="43.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="24.26"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="1" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>1965</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>23922</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>1997</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>1983</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPágina &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>